<commit_message>
Actualización de descarga de datos para forecast
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\forecast_hnd\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B755E5A3-08BC-4E03-AC1A-B770BB1A4DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E92337-72F4-4526-A9A2-8B0872D33136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="20" windowWidth="19180" windowHeight="11260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="47">
   <si>
     <t>Periodo</t>
   </si>
@@ -109,17 +109,65 @@
     <t>password</t>
   </si>
   <si>
-    <t>example@gmail.com</t>
-  </si>
-  <si>
-    <t>example</t>
+    <t>NCEP-CFSv2,GFDL</t>
+  </si>
+  <si>
+    <t>Can-1,Nasa,GFDL</t>
+  </si>
+  <si>
+    <t>Can-2,GFDL</t>
+  </si>
+  <si>
+    <t>NCEP-CFSv2,GFDL,CCSM4</t>
+  </si>
+  <si>
+    <t>CCSM4,GFDL</t>
+  </si>
+  <si>
+    <t>GFDL,NCEP-CFSv2</t>
+  </si>
+  <si>
+    <t>NCEP-CFSv2, GFDL, CCSM4</t>
+  </si>
+  <si>
+    <t>Can-1,Can-2, GFDL</t>
+  </si>
+  <si>
+    <t>Can-1,GFDL,NASA</t>
+  </si>
+  <si>
+    <t>Can-2, CCSM4</t>
+  </si>
+  <si>
+    <t>Can-1,Can-2,NASA</t>
+  </si>
+  <si>
+    <t>NCEP-CFSv2,ECMWF</t>
+  </si>
+  <si>
+    <t>Can-1,Can-2,ECMWF</t>
+  </si>
+  <si>
+    <t>NCEP-CFSv2, Can-1,ECMWF</t>
+  </si>
+  <si>
+    <t>Can-1,Can-2,GFDL,CCSM4,ECMWF</t>
+  </si>
+  <si>
+    <t>Can-1,Can-2,CCSM4,NASA,ECMWF</t>
+  </si>
+  <si>
+    <t>NASA,ECMWF</t>
+  </si>
+  <si>
+    <t>username@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +185,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -169,14 +224,18 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -485,19 +544,14 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="J11" sqref="J11:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="24.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="24.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="14" width="24.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
@@ -552,40 +606,40 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" t="s">
-        <v>23</v>
+        <v>29</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" t="s">
-        <v>23</v>
+        <v>34</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="L2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" t="s">
-        <v>23</v>
+        <v>41</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="N2" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
@@ -904,37 +958,37 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" t="s">
-        <v>23</v>
+        <v>32</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="J10" t="s">
-        <v>23</v>
-      </c>
-      <c r="K10" t="s">
-        <v>23</v>
+        <v>45</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="L10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M10" t="s">
-        <v>23</v>
+        <v>41</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="N10" t="s">
         <v>23</v>
@@ -1249,108 +1303,108 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18">
+      <c r="A18" s="3">
         <v>0</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="N18" s="2" t="s">
-        <v>29</v>
+      <c r="C18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A19">
+      <c r="A19" s="3">
         <v>3</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" t="s">
-        <v>30</v>
-      </c>
-      <c r="F19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G19" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" t="s">
-        <v>30</v>
-      </c>
-      <c r="I19" t="s">
-        <v>30</v>
-      </c>
-      <c r="J19" t="s">
-        <v>30</v>
-      </c>
-      <c r="K19" t="s">
-        <v>30</v>
-      </c>
-      <c r="L19" t="s">
-        <v>30</v>
-      </c>
-      <c r="M19" t="s">
-        <v>30</v>
-      </c>
-      <c r="N19" t="s">
-        <v>30</v>
+      <c r="C19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N19" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C18" r:id="rId1" xr:uid="{A18973F5-68BC-44A3-9976-92762EA58B88}"/>
-    <hyperlink ref="D18" r:id="rId2" xr:uid="{BAD20A6E-9D2F-4AB0-AF08-EA9881798857}"/>
-    <hyperlink ref="E18" r:id="rId3" xr:uid="{A449FDC2-94AD-45DC-A782-CE0FF64D6ECC}"/>
-    <hyperlink ref="F18" r:id="rId4" xr:uid="{E4B528D4-AE8F-4D00-90E9-E56F96B80215}"/>
-    <hyperlink ref="G18" r:id="rId5" xr:uid="{3241B83E-8C94-4EB1-9FD6-0E2A7CE08F6B}"/>
-    <hyperlink ref="H18" r:id="rId6" xr:uid="{56BB1B0E-4585-427E-861D-B63A575A215F}"/>
-    <hyperlink ref="I18" r:id="rId7" xr:uid="{28172737-D822-4C9F-B001-34EA521A5ECE}"/>
-    <hyperlink ref="K18" r:id="rId8" xr:uid="{55D1D252-C2C6-4921-9D8C-BB33F8087EE8}"/>
-    <hyperlink ref="L18" r:id="rId9" xr:uid="{83269A7C-6660-4CF9-BA6A-E8F63376393E}"/>
-    <hyperlink ref="M18" r:id="rId10" xr:uid="{2BB59617-6114-4BF9-B665-76ACA6BF51D1}"/>
-    <hyperlink ref="N18" r:id="rId11" xr:uid="{60D0523E-78BE-4270-B2B7-C71BA0C9D77D}"/>
-    <hyperlink ref="J18" r:id="rId12" xr:uid="{98E7878F-FB04-4238-B991-A2C0D691A71B}"/>
+    <hyperlink ref="C18" r:id="rId1" xr:uid="{BEFBAD75-B794-4156-A824-2B485937EF66}"/>
+    <hyperlink ref="D18" r:id="rId2" xr:uid="{DE539331-29E3-42ED-A210-AB12D7DB82E1}"/>
+    <hyperlink ref="E18" r:id="rId3" xr:uid="{73AF6A30-BC8F-4119-BACC-A6ABA0251DF5}"/>
+    <hyperlink ref="F18" r:id="rId4" xr:uid="{E0B9BFDB-1244-4AFC-9625-FE66EE969152}"/>
+    <hyperlink ref="G18" r:id="rId5" xr:uid="{60232821-C2AA-49EF-B1A2-CB4E50BEEFC6}"/>
+    <hyperlink ref="H18" r:id="rId6" xr:uid="{FF2EFD3F-C5F2-473B-8F64-01F7D2E48C1C}"/>
+    <hyperlink ref="I18" r:id="rId7" xr:uid="{68F68D6E-44B7-4822-9E50-DA967FE6445E}"/>
+    <hyperlink ref="J18" r:id="rId8" xr:uid="{368BA898-A8C8-4D29-8F8A-BF84033F9611}"/>
+    <hyperlink ref="K18" r:id="rId9" xr:uid="{86720E92-DCB5-497F-8BC7-C20BB3473289}"/>
+    <hyperlink ref="L18" r:id="rId10" xr:uid="{41C2332B-08BA-4C9C-839E-D15DCE849C6D}"/>
+    <hyperlink ref="M18" r:id="rId11" xr:uid="{4B5901EC-457D-4BC0-BFA7-26F3D64F2FDE}"/>
+    <hyperlink ref="N18" r:id="rId12" xr:uid="{E5EB86E2-9678-46E4-82D4-4F54B0C1E665}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>